<commit_message>
Removed "No working fire extinguisher" from code list per MLRI feedback.
</commit_message>
<xml_diff>
--- a/docassemble/HousingCodeChecklist/data/templates/housing_code_checklist.xlsx
+++ b/docassemble/HousingCodeChecklist/data/templates/housing_code_checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Keliza/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F13CFFEE-75C8-3D41-A13B-E23702819DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43440ABA-1BF0-714D-8333-1DDC30412A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="tabula-lt1-booklet-2-housing-co" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'tabula-lt1-booklet-2-housing-co'!$A$1:$I$165</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'tabula-lt1-booklet-2-housing-co'!$A$1:$I$164</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1321" uniqueCount="822">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1313" uniqueCount="816">
   <si>
     <t>ID</t>
   </si>
@@ -2010,34 +2010,6 @@
         <family val="2"/>
       </rPr>
       <t>Debe haber electricidad.</t>
-    </r>
-  </si>
-  <si>
-    <t>no_extinguisher</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>No hay extintores de incendios que funcionen</t>
-    </r>
-  </si>
-  <si>
-    <t>The landlord must install and maintain fire extinguishers as required by the local fire chief.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>El dueño debe instalar y mantener los extintores de incendios según de acuerdo con los requisitos del jefe de bomberos local.</t>
     </r>
   </si>
   <si>
@@ -3881,9 +3853,6 @@
     <t>105 C.M.R. 410.140, 410, 630(A)(13)</t>
   </si>
   <si>
-    <t>527 C.M.R. 1.00</t>
-  </si>
-  <si>
     <t>105 C.M.R. 410.310, G.L. c. 143, § 21D</t>
   </si>
   <si>
@@ -4252,9 +4221,6 @@
   </si>
   <si>
     <t>No working carbon monoxide detector.</t>
-  </si>
-  <si>
-    <t>No working fire extinguishers.</t>
   </si>
   <si>
     <t>No working smoke detectors.</t>
@@ -4691,63 +4657,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="14">
     <dxf>
       <fill>
         <patternFill>
@@ -5057,11 +4967,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA361"/>
+  <dimension ref="A1:AA360"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A27" sqref="A26:XFD27"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G73" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -5136,7 +5046,7 @@
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="7" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>30</v>
@@ -5148,7 +5058,7 @@
         <v>32</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="15" x14ac:dyDescent="0.2">
@@ -5163,7 +5073,7 @@
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>34</v>
@@ -5175,7 +5085,7 @@
         <v>36</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>789</v>
+        <v>783</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="15" x14ac:dyDescent="0.2">
@@ -5190,7 +5100,7 @@
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>21</v>
@@ -5202,7 +5112,7 @@
         <v>23</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="15" x14ac:dyDescent="0.2">
@@ -5217,7 +5127,7 @@
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>26</v>
@@ -5229,7 +5139,7 @@
         <v>28</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="15" x14ac:dyDescent="0.2">
@@ -5244,19 +5154,19 @@
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7" t="s">
-        <v>726</v>
+        <v>720</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>46</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>763</v>
+        <v>757</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>47</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="15" x14ac:dyDescent="0.2">
@@ -5271,7 +5181,7 @@
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7" t="s">
-        <v>817</v>
+        <v>811</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>149</v>
@@ -5283,12 +5193,12 @@
         <v>151</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>790</v>
+        <v>784</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>25</v>
@@ -5298,24 +5208,24 @@
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7" t="s">
-        <v>727</v>
+        <v>721</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>791</v>
+        <v>785</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>25</v>
@@ -5325,24 +5235,24 @@
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>25</v>
@@ -5352,24 +5262,24 @@
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>25</v>
@@ -5379,24 +5289,24 @@
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>752</v>
+        <v>746</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>25</v>
@@ -5406,24 +5316,24 @@
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>25</v>
@@ -5433,24 +5343,24 @@
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>753</v>
+        <v>747</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>25</v>
@@ -5460,24 +5370,24 @@
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>25</v>
@@ -5487,34 +5397,34 @@
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>781</v>
+        <v>775</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>820</v>
+        <v>814</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7" t="s">
-        <v>666</v>
+        <v>661</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>60</v>
@@ -5526,22 +5436,22 @@
         <v>62</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
     </row>
     <row r="17" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>779</v>
+        <v>773</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>820</v>
+        <v>814</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7" t="s">
-        <v>658</v>
+        <v>653</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>125</v>
@@ -5553,22 +5463,22 @@
         <v>127</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>792</v>
+        <v>786</v>
       </c>
     </row>
     <row r="18" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>786</v>
+        <v>780</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>820</v>
+        <v>814</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="7" t="s">
-        <v>744</v>
+        <v>738</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>154</v>
@@ -5580,130 +5490,130 @@
         <v>156</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>793</v>
+        <v>787</v>
       </c>
     </row>
     <row r="19" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>820</v>
+        <v>814</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7" t="s">
-        <v>821</v>
+        <v>815</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>264</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>819</v>
+        <v>813</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>266</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
     </row>
     <row r="20" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>785</v>
+        <v>779</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>820</v>
+        <v>814</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="7" t="s">
-        <v>701</v>
+        <v>696</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
     </row>
     <row r="21" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>783</v>
+        <v>777</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>820</v>
+        <v>814</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="7" t="s">
-        <v>676</v>
+        <v>671</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
     </row>
     <row r="22" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>780</v>
+        <v>774</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>820</v>
+        <v>814</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="7" t="s">
-        <v>663</v>
+        <v>658</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>794</v>
+        <v>788</v>
       </c>
     </row>
     <row r="23" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>782</v>
+        <v>776</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>820</v>
+        <v>814</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="7" t="s">
-        <v>670</v>
+        <v>665</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>137</v>
@@ -5715,49 +5625,49 @@
         <v>139</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
     </row>
     <row r="24" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>787</v>
+        <v>781</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>820</v>
+        <v>814</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="7" t="s">
-        <v>720</v>
+        <v>714</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>795</v>
+        <v>789</v>
       </c>
     </row>
     <row r="25" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>788</v>
+        <v>782</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>820</v>
+        <v>814</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="7" t="s">
-        <v>722</v>
+        <v>716</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>145</v>
@@ -5769,103 +5679,103 @@
         <v>147</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>796</v>
+        <v>790</v>
       </c>
     </row>
     <row r="26" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>772</v>
+        <v>766</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>820</v>
+        <v>814</v>
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="7" t="s">
-        <v>729</v>
+        <v>723</v>
       </c>
       <c r="F26" s="7" t="s">
         <v>106</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>764</v>
+        <v>758</v>
       </c>
       <c r="H26" s="7" t="s">
         <v>107</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
     </row>
     <row r="27" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
-        <v>773</v>
+        <v>767</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>820</v>
+        <v>814</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="7" t="s">
-        <v>728</v>
+        <v>722</v>
       </c>
       <c r="F27" s="7" t="s">
         <v>64</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>766</v>
+        <v>760</v>
       </c>
       <c r="H27" s="7" t="s">
         <v>65</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
     </row>
     <row r="28" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>774</v>
+        <v>768</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>820</v>
+        <v>814</v>
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="7" t="s">
-        <v>731</v>
+        <v>725</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>767</v>
+        <v>761</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
     </row>
     <row r="29" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>778</v>
+        <v>772</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>820</v>
+        <v>814</v>
       </c>
       <c r="D29" s="7"/>
       <c r="E29" s="7" t="s">
-        <v>657</v>
+        <v>652</v>
       </c>
       <c r="F29" s="7" t="s">
         <v>102</v>
@@ -5877,22 +5787,22 @@
         <v>104</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
     </row>
     <row r="30" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>775</v>
+        <v>769</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>820</v>
+        <v>814</v>
       </c>
       <c r="D30" s="7"/>
       <c r="E30" s="7" t="s">
-        <v>734</v>
+        <v>728</v>
       </c>
       <c r="F30" s="7" t="s">
         <v>70</v>
@@ -5904,61 +5814,61 @@
         <v>72</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="31" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>776</v>
+        <v>770</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>820</v>
+        <v>814</v>
       </c>
       <c r="D31" s="7"/>
       <c r="E31" s="7" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
       <c r="F31" s="7" t="s">
         <v>112</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="H31" s="7" t="s">
         <v>113</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="32" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>777</v>
+        <v>771</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>820</v>
+        <v>814</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="7" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="J32" s="7"/>
       <c r="K32" s="7"/>
@@ -5990,19 +5900,19 @@
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="7" t="s">
-        <v>726</v>
+        <v>720</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>39</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="H33" s="7" t="s">
         <v>40</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="34" spans="1:26" ht="15" x14ac:dyDescent="0.2">
@@ -6017,19 +5927,19 @@
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="7" t="s">
-        <v>728</v>
+        <v>722</v>
       </c>
       <c r="F34" s="7" t="s">
         <v>64</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>766</v>
+        <v>760</v>
       </c>
       <c r="H34" s="7" t="s">
         <v>65</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
     </row>
     <row r="35" spans="1:26" ht="15" x14ac:dyDescent="0.2">
@@ -6044,19 +5954,19 @@
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="7" t="s">
-        <v>729</v>
+        <v>723</v>
       </c>
       <c r="F35" s="7" t="s">
         <v>106</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>764</v>
+        <v>758</v>
       </c>
       <c r="H35" s="7" t="s">
         <v>107</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
     </row>
     <row r="36" spans="1:26" ht="15" x14ac:dyDescent="0.2">
@@ -6064,26 +5974,26 @@
         <v>184</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>38</v>
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="7" t="s">
-        <v>730</v>
+        <v>724</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="H36" s="7" t="s">
         <v>185</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
     </row>
     <row r="37" spans="1:26" ht="15" x14ac:dyDescent="0.2">
@@ -6098,7 +6008,7 @@
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="7" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="F37" s="7" t="s">
         <v>241</v>
@@ -6110,12 +6020,12 @@
         <v>242</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>798</v>
+        <v>792</v>
       </c>
     </row>
     <row r="38" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>25</v>
@@ -6125,24 +6035,24 @@
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="7" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>754</v>
+        <v>748</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
     </row>
     <row r="39" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>25</v>
@@ -6152,24 +6062,24 @@
       </c>
       <c r="D39" s="7"/>
       <c r="E39" s="7" t="s">
-        <v>731</v>
+        <v>725</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>767</v>
+        <v>761</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
     </row>
     <row r="40" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>25</v>
@@ -6179,24 +6089,24 @@
       </c>
       <c r="D40" s="7"/>
       <c r="E40" s="7" t="s">
-        <v>732</v>
+        <v>726</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
     </row>
     <row r="41" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>25</v>
@@ -6206,19 +6116,19 @@
       </c>
       <c r="D41" s="7"/>
       <c r="E41" s="7" t="s">
-        <v>733</v>
+        <v>727</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
     </row>
     <row r="42" spans="1:26" ht="15" x14ac:dyDescent="0.2">
@@ -6233,7 +6143,7 @@
       </c>
       <c r="D42" s="7"/>
       <c r="E42" s="7" t="s">
-        <v>734</v>
+        <v>728</v>
       </c>
       <c r="F42" s="7" t="s">
         <v>70</v>
@@ -6245,7 +6155,7 @@
         <v>72</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="43" spans="1:26" ht="15" x14ac:dyDescent="0.2">
@@ -6260,7 +6170,7 @@
       </c>
       <c r="D43" s="7"/>
       <c r="E43" s="7" t="s">
-        <v>735</v>
+        <v>729</v>
       </c>
       <c r="F43" s="7" t="s">
         <v>74</v>
@@ -6272,7 +6182,7 @@
         <v>76</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="44" spans="1:26" ht="15" x14ac:dyDescent="0.2">
@@ -6287,19 +6197,19 @@
       </c>
       <c r="D44" s="7"/>
       <c r="E44" s="7" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
       <c r="F44" s="7" t="s">
         <v>52</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="H44" s="7" t="s">
         <v>53</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="45" spans="1:26" ht="15" x14ac:dyDescent="0.2">
@@ -6314,7 +6224,7 @@
       </c>
       <c r="D45" s="7"/>
       <c r="E45" s="7" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
       <c r="F45" s="7" t="s">
         <v>78</v>
@@ -6326,7 +6236,7 @@
         <v>80</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
     </row>
     <row r="46" spans="1:26" ht="15" x14ac:dyDescent="0.2">
@@ -6341,7 +6251,7 @@
       </c>
       <c r="D46" s="7"/>
       <c r="E46" s="7" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
       <c r="F46" s="7" t="s">
         <v>82</v>
@@ -6353,7 +6263,7 @@
         <v>84</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
     </row>
     <row r="47" spans="1:26" ht="15" x14ac:dyDescent="0.2">
@@ -6368,24 +6278,24 @@
       </c>
       <c r="D47" s="7"/>
       <c r="E47" s="7" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
       <c r="F47" s="7" t="s">
         <v>112</v>
       </c>
       <c r="G47" s="10" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="H47" s="7" t="s">
         <v>113</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="48" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>25</v>
@@ -6395,19 +6305,19 @@
       </c>
       <c r="D48" s="7"/>
       <c r="E48" s="7" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="G48" s="10" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="J48" s="7"/>
       <c r="K48" s="7"/>
@@ -6429,7 +6339,7 @@
     </row>
     <row r="49" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>25</v>
@@ -6439,24 +6349,24 @@
       </c>
       <c r="D49" s="7"/>
       <c r="E49" s="7" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>797</v>
+        <v>791</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>25</v>
@@ -6466,24 +6376,24 @@
       </c>
       <c r="D50" s="7"/>
       <c r="E50" s="7" t="s">
-        <v>641</v>
+        <v>636</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="G50" s="10" t="s">
+        <v>435</v>
+      </c>
+      <c r="H50" s="7" t="s">
         <v>439</v>
       </c>
-      <c r="H50" s="7" t="s">
-        <v>443</v>
-      </c>
       <c r="I50" s="2" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>25</v>
@@ -6493,19 +6403,19 @@
       </c>
       <c r="D51" s="7"/>
       <c r="E51" s="7" t="s">
-        <v>642</v>
+        <v>637</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="G51" s="10" t="s">
-        <v>755</v>
+        <v>749</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -6520,7 +6430,7 @@
       </c>
       <c r="D52" s="7"/>
       <c r="E52" s="7" t="s">
-        <v>643</v>
+        <v>638</v>
       </c>
       <c r="F52" s="7" t="s">
         <v>280</v>
@@ -6532,12 +6442,12 @@
         <v>282</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>799</v>
+        <v>793</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>25</v>
@@ -6547,19 +6457,19 @@
       </c>
       <c r="D53" s="7"/>
       <c r="E53" s="7" t="s">
-        <v>644</v>
+        <v>639</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>799</v>
+        <v>793</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -6567,14 +6477,14 @@
         <v>157</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>158</v>
       </c>
       <c r="D54" s="7"/>
       <c r="E54" s="7" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="F54" s="7" t="s">
         <v>159</v>
@@ -6586,7 +6496,7 @@
         <v>161</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -6601,19 +6511,19 @@
       </c>
       <c r="D55" s="7"/>
       <c r="E55" s="7" t="s">
-        <v>736</v>
+        <v>730</v>
       </c>
       <c r="F55" s="7" t="s">
         <v>179</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>756</v>
+        <v>750</v>
       </c>
       <c r="H55" s="7" t="s">
         <v>180</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -6628,7 +6538,7 @@
       </c>
       <c r="D56" s="7"/>
       <c r="E56" s="7" t="s">
-        <v>646</v>
+        <v>641</v>
       </c>
       <c r="F56" s="7" t="s">
         <v>175</v>
@@ -6640,7 +6550,7 @@
         <v>177</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -6648,14 +6558,14 @@
         <v>275</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>158</v>
       </c>
       <c r="D57" s="7"/>
       <c r="E57" s="7" t="s">
-        <v>647</v>
+        <v>642</v>
       </c>
       <c r="F57" s="7" t="s">
         <v>276</v>
@@ -6667,66 +6577,66 @@
         <v>278</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>799</v>
+        <v>793</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="C58" s="7" t="s">
         <v>158</v>
       </c>
       <c r="D58" s="7"/>
       <c r="E58" s="7" t="s">
-        <v>648</v>
+        <v>643</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="G58" s="10" t="s">
         <v>277</v>
       </c>
       <c r="H58" s="7" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>799</v>
+        <v>793</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="C59" s="7" t="s">
         <v>158</v>
       </c>
       <c r="D59" s="7"/>
       <c r="E59" s="7" t="s">
-        <v>649</v>
+        <v>644</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="G59" s="10" t="s">
         <v>277</v>
       </c>
       <c r="H59" s="7" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>799</v>
+        <v>793</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B60" s="7" t="s">
         <v>25</v>
@@ -6736,24 +6646,24 @@
       </c>
       <c r="D60" s="7"/>
       <c r="E60" s="7" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="H60" s="7" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>25</v>
@@ -6763,24 +6673,24 @@
       </c>
       <c r="D61" s="7"/>
       <c r="E61" s="7" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="H61" s="7" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>25</v>
@@ -6790,24 +6700,24 @@
       </c>
       <c r="D62" s="7"/>
       <c r="E62" s="7" t="s">
-        <v>652</v>
+        <v>647</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="H62" s="7" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B63" s="7" t="s">
         <v>25</v>
@@ -6817,24 +6727,24 @@
       </c>
       <c r="D63" s="7"/>
       <c r="E63" s="7" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="G63" s="10" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="H63" s="7" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="B64" s="7" t="s">
         <v>25</v>
@@ -6844,24 +6754,24 @@
       </c>
       <c r="D64" s="7"/>
       <c r="E64" s="7" t="s">
-        <v>654</v>
+        <v>649</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="G64" s="10" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="H64" s="7" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>800</v>
+        <v>794</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="B65" s="7" t="s">
         <v>25</v>
@@ -6871,19 +6781,19 @@
       </c>
       <c r="D65" s="7"/>
       <c r="E65" s="7" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="G65" s="10" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="H65" s="7" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>800</v>
+        <v>794</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -6898,7 +6808,7 @@
       </c>
       <c r="D66" s="7"/>
       <c r="E66" s="7" t="s">
-        <v>656</v>
+        <v>651</v>
       </c>
       <c r="F66" s="7" t="s">
         <v>94</v>
@@ -6910,7 +6820,7 @@
         <v>96</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>800</v>
+        <v>794</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -6918,14 +6828,14 @@
         <v>97</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="C67" s="7" t="s">
         <v>93</v>
       </c>
       <c r="D67" s="7"/>
       <c r="E67" s="7" t="s">
-        <v>801</v>
+        <v>795</v>
       </c>
       <c r="F67" s="7" t="s">
         <v>98</v>
@@ -6937,7 +6847,7 @@
         <v>100</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -6952,7 +6862,7 @@
       </c>
       <c r="D68" s="7"/>
       <c r="E68" s="7" t="s">
-        <v>657</v>
+        <v>652</v>
       </c>
       <c r="F68" s="7" t="s">
         <v>102</v>
@@ -6964,7 +6874,7 @@
         <v>104</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -6979,7 +6889,7 @@
       </c>
       <c r="D69" s="7"/>
       <c r="E69" s="7" t="s">
-        <v>658</v>
+        <v>653</v>
       </c>
       <c r="F69" s="7" t="s">
         <v>125</v>
@@ -6991,7 +6901,7 @@
         <v>127</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>792</v>
+        <v>786</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -7006,24 +6916,24 @@
       </c>
       <c r="D70" s="7"/>
       <c r="E70" s="7" t="s">
-        <v>659</v>
+        <v>654</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="G70" s="10" t="s">
-        <v>757</v>
+        <v>751</v>
       </c>
       <c r="H70" s="7" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="I70" s="2" t="s">
-        <v>792</v>
+        <v>786</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A71" s="7" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="B71" s="13" t="s">
         <v>25</v>
@@ -7033,19 +6943,19 @@
       </c>
       <c r="D71" s="7"/>
       <c r="E71" s="7" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="G71" s="10" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="H71" s="7" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>792</v>
+        <v>786</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -7053,14 +6963,14 @@
         <v>88</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="C72" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D72" s="7"/>
       <c r="E72" s="7" t="s">
-        <v>661</v>
+        <v>656</v>
       </c>
       <c r="F72" s="7" t="s">
         <v>89</v>
@@ -7072,12 +6982,12 @@
         <v>91</v>
       </c>
       <c r="I72" s="2" t="s">
-        <v>802</v>
+        <v>796</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A73" s="7" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="B73" s="7" t="s">
         <v>25</v>
@@ -7087,24 +6997,24 @@
       </c>
       <c r="D73" s="7"/>
       <c r="E73" s="7" t="s">
-        <v>662</v>
+        <v>657</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="G73" s="10" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="H73" s="7" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="I73" s="2" t="s">
-        <v>802</v>
+        <v>796</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A74" s="7" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="B74" s="7" t="s">
         <v>25</v>
@@ -7114,24 +7024,24 @@
       </c>
       <c r="D74" s="7"/>
       <c r="E74" s="7" t="s">
-        <v>663</v>
+        <v>658</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="G74" s="10" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="H74" s="7" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="I74" s="2" t="s">
-        <v>794</v>
+        <v>788</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A75" s="7" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="B75" s="7" t="s">
         <v>25</v>
@@ -7141,19 +7051,19 @@
       </c>
       <c r="D75" s="7"/>
       <c r="E75" s="7" t="s">
-        <v>664</v>
+        <v>659</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="G75" s="10" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="H75" s="7" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -7161,14 +7071,14 @@
         <v>9</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="C76" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D76" s="7"/>
       <c r="E76" s="7" t="s">
-        <v>665</v>
+        <v>660</v>
       </c>
       <c r="F76" s="7" t="s">
         <v>11</v>
@@ -7180,7 +7090,7 @@
         <v>13</v>
       </c>
       <c r="I76" s="2" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -7195,7 +7105,7 @@
       </c>
       <c r="D77" s="7"/>
       <c r="E77" s="7" t="s">
-        <v>666</v>
+        <v>661</v>
       </c>
       <c r="F77" s="7" t="s">
         <v>60</v>
@@ -7207,7 +7117,7 @@
         <v>62</v>
       </c>
       <c r="I77" s="2" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -7215,26 +7125,26 @@
         <v>85</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="C78" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D78" s="7"/>
       <c r="E78" s="7" t="s">
-        <v>667</v>
+        <v>662</v>
       </c>
       <c r="F78" s="7" t="s">
         <v>86</v>
       </c>
       <c r="G78" s="10" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="H78" s="7" t="s">
         <v>87</v>
       </c>
       <c r="I78" s="2" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -7249,7 +7159,7 @@
       </c>
       <c r="D79" s="7"/>
       <c r="E79" s="7" t="s">
-        <v>668</v>
+        <v>663</v>
       </c>
       <c r="F79" s="7" t="s">
         <v>129</v>
@@ -7261,7 +7171,7 @@
         <v>131</v>
       </c>
       <c r="I79" s="2" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -7269,14 +7179,14 @@
         <v>132</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="C80" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D80" s="7"/>
       <c r="E80" s="7" t="s">
-        <v>669</v>
+        <v>664</v>
       </c>
       <c r="F80" s="7" t="s">
         <v>133</v>
@@ -7288,7 +7198,7 @@
         <v>135</v>
       </c>
       <c r="I80" s="2" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -7303,7 +7213,7 @@
       </c>
       <c r="D81" s="7"/>
       <c r="E81" s="7" t="s">
-        <v>670</v>
+        <v>665</v>
       </c>
       <c r="F81" s="7" t="s">
         <v>137</v>
@@ -7315,169 +7225,169 @@
         <v>139</v>
       </c>
       <c r="I81" s="2" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A82" s="7" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="C82" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D82" s="7"/>
       <c r="E82" s="7" t="s">
-        <v>671</v>
+        <v>666</v>
       </c>
       <c r="F82" s="7" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="G82" s="10" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="H82" s="7" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="I82" s="2" t="s">
-        <v>803</v>
+        <v>797</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A83" s="7" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="C83" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D83" s="7"/>
       <c r="E83" s="7" t="s">
-        <v>672</v>
+        <v>667</v>
       </c>
       <c r="F83" s="7" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="G83" s="10" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="H83" s="7" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="I83" s="2" t="s">
-        <v>804</v>
+        <v>798</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A84" s="7" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="C84" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D84" s="7"/>
       <c r="E84" s="7" t="s">
-        <v>673</v>
+        <v>668</v>
       </c>
       <c r="F84" s="7" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="G84" s="10" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="H84" s="7" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="I84" s="2" t="s">
-        <v>804</v>
+        <v>798</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="C85" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D85" s="7"/>
       <c r="E85" s="7" t="s">
-        <v>674</v>
+        <v>669</v>
       </c>
       <c r="F85" s="7" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="G85" s="10" t="s">
-        <v>768</v>
+        <v>762</v>
       </c>
       <c r="H85" s="7" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="I85" s="2" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="C86" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D86" s="7"/>
       <c r="E86" s="7" t="s">
-        <v>675</v>
+        <v>670</v>
       </c>
       <c r="F86" s="7" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="G86" s="10" t="s">
-        <v>769</v>
+        <v>763</v>
       </c>
       <c r="H86" s="7" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="I86" s="2" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="C87" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D87" s="7"/>
       <c r="E87" s="7" t="s">
-        <v>676</v>
+        <v>671</v>
       </c>
       <c r="F87" s="7" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="G87" s="10" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="H87" s="7" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="I87" s="2" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -7492,19 +7402,19 @@
       </c>
       <c r="D88" s="7"/>
       <c r="E88" s="7" t="s">
-        <v>737</v>
+        <v>731</v>
       </c>
       <c r="F88" s="7" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="G88" s="11" t="s">
-        <v>758</v>
+        <v>752</v>
       </c>
       <c r="H88" s="8" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="I88" s="2" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -7519,7 +7429,7 @@
       </c>
       <c r="D89" s="7"/>
       <c r="E89" s="7" t="s">
-        <v>677</v>
+        <v>672</v>
       </c>
       <c r="F89" s="7" t="s">
         <v>120</v>
@@ -7531,7 +7441,7 @@
         <v>122</v>
       </c>
       <c r="I89" s="2" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -7546,10 +7456,10 @@
       </c>
       <c r="D90" s="7"/>
       <c r="E90" s="7" t="s">
-        <v>678</v>
+        <v>673</v>
       </c>
       <c r="F90" s="7" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="G90" s="10" t="s">
         <v>142</v>
@@ -7558,7 +7468,7 @@
         <v>143</v>
       </c>
       <c r="I90" s="2" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -7566,14 +7476,14 @@
         <v>223</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="C91" s="7" t="s">
         <v>119</v>
       </c>
       <c r="D91" s="7"/>
       <c r="E91" s="7" t="s">
-        <v>738</v>
+        <v>732</v>
       </c>
       <c r="F91" s="7" t="s">
         <v>224</v>
@@ -7585,12 +7495,12 @@
         <v>226</v>
       </c>
       <c r="I91" s="2" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A92" s="7" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B92" s="7" t="s">
         <v>25</v>
@@ -7600,24 +7510,24 @@
       </c>
       <c r="D92" s="7"/>
       <c r="E92" s="7" t="s">
-        <v>679</v>
+        <v>674</v>
       </c>
       <c r="F92" s="7" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="G92" s="10" t="s">
-        <v>759</v>
+        <v>753</v>
       </c>
       <c r="H92" s="7" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="I92" s="2" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
     </row>
     <row r="93" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A93" s="7" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B93" s="7" t="s">
         <v>25</v>
@@ -7627,24 +7537,24 @@
       </c>
       <c r="D93" s="7"/>
       <c r="E93" s="7" t="s">
-        <v>680</v>
+        <v>675</v>
       </c>
       <c r="F93" s="7" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G93" s="10" t="s">
-        <v>760</v>
+        <v>754</v>
       </c>
       <c r="H93" s="7" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="I93" s="2" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A94" s="7" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B94" s="7" t="s">
         <v>25</v>
@@ -7654,24 +7564,24 @@
       </c>
       <c r="D94" s="7"/>
       <c r="E94" s="7" t="s">
-        <v>681</v>
+        <v>676</v>
       </c>
       <c r="F94" s="7" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="G94" s="10" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="H94" s="7" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="I94" s="2" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A95" s="7" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="B95" s="7" t="s">
         <v>25</v>
@@ -7681,24 +7591,24 @@
       </c>
       <c r="D95" s="7"/>
       <c r="E95" s="7" t="s">
-        <v>682</v>
+        <v>677</v>
       </c>
       <c r="F95" s="7" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="G95" s="10" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="H95" s="7" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="I95" s="2" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
     </row>
     <row r="96" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A96" s="7" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="B96" s="7" t="s">
         <v>25</v>
@@ -7708,24 +7618,24 @@
       </c>
       <c r="D96" s="7"/>
       <c r="E96" s="7" t="s">
-        <v>683</v>
+        <v>678</v>
       </c>
       <c r="F96" s="7" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="G96" s="10" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="H96" s="7" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="I96" s="2" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
     </row>
     <row r="97" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A97" s="7" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B97" s="7" t="s">
         <v>25</v>
@@ -7735,24 +7645,24 @@
       </c>
       <c r="D97" s="7"/>
       <c r="E97" s="7" t="s">
-        <v>739</v>
+        <v>733</v>
       </c>
       <c r="F97" s="7" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="G97" s="10" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="H97" s="7" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="I97" s="2" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
     </row>
     <row r="98" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A98" s="7" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="B98" s="7" t="s">
         <v>25</v>
@@ -7762,19 +7672,19 @@
       </c>
       <c r="D98" s="7"/>
       <c r="E98" s="7" t="s">
-        <v>684</v>
+        <v>679</v>
       </c>
       <c r="F98" s="7" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="G98" s="10" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="H98" s="7" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="I98" s="2" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
     </row>
     <row r="99" spans="1:26" ht="15" x14ac:dyDescent="0.2">
@@ -7789,7 +7699,7 @@
       </c>
       <c r="D99" s="7"/>
       <c r="E99" s="7" t="s">
-        <v>685</v>
+        <v>680</v>
       </c>
       <c r="F99" s="7" t="s">
         <v>215</v>
@@ -7801,7 +7711,7 @@
         <v>217</v>
       </c>
       <c r="I99" s="2" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
     </row>
     <row r="100" spans="1:26" ht="15" x14ac:dyDescent="0.2">
@@ -7816,7 +7726,7 @@
       </c>
       <c r="D100" s="7"/>
       <c r="E100" s="7" t="s">
-        <v>686</v>
+        <v>681</v>
       </c>
       <c r="F100" s="7" t="s">
         <v>219</v>
@@ -7828,12 +7738,12 @@
         <v>221</v>
       </c>
       <c r="I100" s="2" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
     </row>
     <row r="101" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A101" s="7" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B101" s="7" t="s">
         <v>25</v>
@@ -7843,19 +7753,19 @@
       </c>
       <c r="D101" s="7"/>
       <c r="E101" s="7" t="s">
-        <v>687</v>
+        <v>682</v>
       </c>
       <c r="F101" s="7" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="G101" s="10" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="H101" s="7" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="I101" s="2" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
     </row>
     <row r="102" spans="1:26" ht="15" x14ac:dyDescent="0.2">
@@ -7870,7 +7780,7 @@
       </c>
       <c r="D102" s="7"/>
       <c r="E102" s="7" t="s">
-        <v>688</v>
+        <v>683</v>
       </c>
       <c r="F102" s="7" t="s">
         <v>17</v>
@@ -7882,12 +7792,12 @@
         <v>19</v>
       </c>
       <c r="I102" s="2" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
     </row>
     <row r="103" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A103" s="7" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="B103" s="7" t="s">
         <v>25</v>
@@ -7897,19 +7807,19 @@
       </c>
       <c r="D103" s="7"/>
       <c r="E103" s="7" t="s">
-        <v>689</v>
+        <v>684</v>
       </c>
       <c r="F103" s="7" t="s">
         <v>48</v>
       </c>
       <c r="G103" s="10" t="s">
-        <v>763</v>
+        <v>757</v>
       </c>
       <c r="H103" s="7" t="s">
         <v>49</v>
       </c>
       <c r="I103" s="2" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="104" spans="1:26" ht="15" x14ac:dyDescent="0.2">
@@ -7917,14 +7827,14 @@
         <v>199</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="C104" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D104" s="7"/>
       <c r="E104" s="7" t="s">
-        <v>690</v>
+        <v>685</v>
       </c>
       <c r="F104" s="7" t="s">
         <v>200</v>
@@ -7936,7 +7846,7 @@
         <v>202</v>
       </c>
       <c r="I104" s="2" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
     </row>
     <row r="105" spans="1:26" ht="15" x14ac:dyDescent="0.2">
@@ -7944,14 +7854,14 @@
         <v>203</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="C105" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D105" s="7"/>
       <c r="E105" s="7" t="s">
-        <v>691</v>
+        <v>686</v>
       </c>
       <c r="F105" s="7" t="s">
         <v>204</v>
@@ -7963,7 +7873,7 @@
         <v>206</v>
       </c>
       <c r="I105" s="2" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
     </row>
     <row r="106" spans="1:26" ht="15" x14ac:dyDescent="0.2">
@@ -7978,19 +7888,19 @@
       </c>
       <c r="D106" s="7"/>
       <c r="E106" s="7" t="s">
-        <v>692</v>
+        <v>687</v>
       </c>
       <c r="F106" s="7" t="s">
         <v>208</v>
       </c>
       <c r="G106" s="10" t="s">
-        <v>770</v>
+        <v>764</v>
       </c>
       <c r="H106" s="7" t="s">
         <v>209</v>
       </c>
       <c r="I106" s="2" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
     </row>
     <row r="107" spans="1:26" ht="15" x14ac:dyDescent="0.2">
@@ -8005,7 +7915,7 @@
       </c>
       <c r="D107" s="7"/>
       <c r="E107" s="7" t="s">
-        <v>740</v>
+        <v>734</v>
       </c>
       <c r="F107" s="7" t="s">
         <v>211</v>
@@ -8017,7 +7927,7 @@
         <v>213</v>
       </c>
       <c r="I107" s="2" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="J107" s="7"/>
       <c r="K107" s="7"/>
@@ -8039,7 +7949,7 @@
     </row>
     <row r="108" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A108" s="7" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B108" s="7" t="s">
         <v>25</v>
@@ -8049,24 +7959,24 @@
       </c>
       <c r="D108" s="7"/>
       <c r="E108" s="7" t="s">
-        <v>693</v>
+        <v>688</v>
       </c>
       <c r="F108" s="7" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="G108" s="10" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="H108" s="7" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="I108" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
     </row>
     <row r="109" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A109" s="7" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B109" s="7" t="s">
         <v>25</v>
@@ -8076,19 +7986,19 @@
       </c>
       <c r="D109" s="7"/>
       <c r="E109" s="7" t="s">
-        <v>694</v>
+        <v>689</v>
       </c>
       <c r="F109" s="7" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="G109" s="10" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="H109" s="7" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="I109" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="J109" s="7"/>
       <c r="K109" s="7"/>
@@ -8110,7 +8020,7 @@
     </row>
     <row r="110" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A110" s="7" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="B110" s="7" t="s">
         <v>25</v>
@@ -8120,73 +8030,73 @@
       </c>
       <c r="D110" s="7"/>
       <c r="E110" s="7" t="s">
-        <v>731</v>
+        <v>725</v>
       </c>
       <c r="F110" s="7" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="G110" s="10" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="H110" s="7" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="I110" s="2" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="111" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A111" s="7" t="s">
+        <v>611</v>
+      </c>
+      <c r="B111" s="7" t="s">
         <v>616</v>
-      </c>
-      <c r="B111" s="7" t="s">
-        <v>621</v>
       </c>
       <c r="C111" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D111" s="7"/>
       <c r="E111" s="7" t="s">
-        <v>695</v>
+        <v>690</v>
       </c>
       <c r="F111" s="7" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="G111" s="10" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="H111" s="7" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="I111" s="2" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="112" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A112" s="7" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="C112" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D112" s="7"/>
       <c r="E112" s="7" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="F112" s="7" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="G112" s="10" t="s">
-        <v>754</v>
+        <v>748</v>
       </c>
       <c r="H112" s="7" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="I112" s="3" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
     </row>
     <row r="113" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -8201,7 +8111,7 @@
       </c>
       <c r="D113" s="7"/>
       <c r="E113" s="7" t="s">
-        <v>696</v>
+        <v>691</v>
       </c>
       <c r="F113" s="7" t="s">
         <v>237</v>
@@ -8213,7 +8123,7 @@
         <v>239</v>
       </c>
       <c r="I113" s="2" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
     </row>
     <row r="114" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -8228,7 +8138,7 @@
       </c>
       <c r="D114" s="8"/>
       <c r="E114" s="8" t="s">
-        <v>697</v>
+        <v>692</v>
       </c>
       <c r="F114" s="8" t="s">
         <v>229</v>
@@ -8240,7 +8150,7 @@
         <v>231</v>
       </c>
       <c r="I114" s="4" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
     </row>
     <row r="115" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -8255,7 +8165,7 @@
       </c>
       <c r="D115" s="7"/>
       <c r="E115" s="7" t="s">
-        <v>698</v>
+        <v>693</v>
       </c>
       <c r="F115" s="7" t="s">
         <v>233</v>
@@ -8267,34 +8177,34 @@
         <v>235</v>
       </c>
       <c r="I115" s="2" t="s">
-        <v>805</v>
+        <v>799</v>
       </c>
     </row>
     <row r="116" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A116" s="7" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="C116" s="7" t="s">
         <v>163</v>
       </c>
       <c r="D116" s="7"/>
       <c r="E116" s="7" t="s">
-        <v>741</v>
+        <v>735</v>
       </c>
       <c r="F116" s="7" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="G116" s="10" t="s">
-        <v>771</v>
+        <v>765</v>
       </c>
       <c r="H116" s="7" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="I116" s="2" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
     </row>
     <row r="117" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -8302,26 +8212,26 @@
         <v>167</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="C117" s="7" t="s">
         <v>163</v>
       </c>
       <c r="D117" s="7"/>
       <c r="E117" s="7" t="s">
-        <v>811</v>
+        <v>805</v>
       </c>
       <c r="F117" s="7" t="s">
         <v>168</v>
       </c>
       <c r="G117" s="10" t="s">
-        <v>812</v>
+        <v>806</v>
       </c>
       <c r="H117" s="7" t="s">
         <v>169</v>
       </c>
       <c r="I117" s="2" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
     </row>
     <row r="118" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -8329,26 +8239,26 @@
         <v>181</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="C118" s="7" t="s">
         <v>163</v>
       </c>
       <c r="D118" s="7"/>
       <c r="E118" s="7" t="s">
-        <v>816</v>
+        <v>810</v>
       </c>
       <c r="F118" s="7" t="s">
         <v>182</v>
       </c>
       <c r="G118" s="10" t="s">
-        <v>813</v>
+        <v>807</v>
       </c>
       <c r="H118" s="7" t="s">
         <v>183</v>
       </c>
       <c r="I118" s="2" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
     </row>
     <row r="119" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -8356,26 +8266,26 @@
         <v>189</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="C119" s="7" t="s">
         <v>163</v>
       </c>
       <c r="D119" s="7"/>
       <c r="E119" s="7" t="s">
-        <v>815</v>
+        <v>809</v>
       </c>
       <c r="F119" s="7" t="s">
         <v>190</v>
       </c>
       <c r="G119" s="10" t="s">
-        <v>814</v>
+        <v>808</v>
       </c>
       <c r="H119" s="7" t="s">
         <v>191</v>
       </c>
       <c r="I119" s="2" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
     </row>
     <row r="120" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -8383,14 +8293,14 @@
         <v>162</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="C120" s="7" t="s">
         <v>163</v>
       </c>
       <c r="D120" s="7"/>
       <c r="E120" s="7" t="s">
-        <v>742</v>
+        <v>736</v>
       </c>
       <c r="F120" s="7" t="s">
         <v>164</v>
@@ -8402,7 +8312,7 @@
         <v>166</v>
       </c>
       <c r="I120" s="2" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
     </row>
     <row r="121" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -8417,7 +8327,7 @@
       </c>
       <c r="D121" s="7"/>
       <c r="E121" s="7" t="s">
-        <v>818</v>
+        <v>812</v>
       </c>
       <c r="F121" s="7" t="s">
         <v>264</v>
@@ -8429,7 +8339,7 @@
         <v>266</v>
       </c>
       <c r="I121" s="2" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
     </row>
     <row r="122" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -8444,7 +8354,7 @@
       </c>
       <c r="D122" s="7"/>
       <c r="E122" s="7" t="s">
-        <v>699</v>
+        <v>694</v>
       </c>
       <c r="F122" s="7" t="s">
         <v>268</v>
@@ -8456,12 +8366,12 @@
         <v>270</v>
       </c>
       <c r="I122" s="2" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
     </row>
     <row r="123" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A123" s="7" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B123" s="7" t="s">
         <v>25</v>
@@ -8471,24 +8381,24 @@
       </c>
       <c r="D123" s="7"/>
       <c r="E123" s="7" t="s">
-        <v>700</v>
+        <v>695</v>
       </c>
       <c r="F123" s="7" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="G123" s="10" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="H123" s="7" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="I123" s="2" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
     </row>
     <row r="124" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A124" s="7" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B124" s="7" t="s">
         <v>25</v>
@@ -8498,24 +8408,24 @@
       </c>
       <c r="D124" s="7"/>
       <c r="E124" s="7" t="s">
-        <v>701</v>
+        <v>696</v>
       </c>
       <c r="F124" s="7" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="G124" s="10" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="H124" s="7" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="I124" s="2" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
     </row>
     <row r="125" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A125" s="7" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B125" s="7" t="s">
         <v>25</v>
@@ -8525,24 +8435,24 @@
       </c>
       <c r="D125" s="7"/>
       <c r="E125" s="7" t="s">
-        <v>702</v>
+        <v>697</v>
       </c>
       <c r="F125" s="7" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="G125" s="10" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="H125" s="7" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="I125" s="2" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
     </row>
     <row r="126" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A126" s="7" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B126" s="7" t="s">
         <v>25</v>
@@ -8552,24 +8462,24 @@
       </c>
       <c r="D126" s="7"/>
       <c r="E126" s="7" t="s">
-        <v>703</v>
+        <v>698</v>
       </c>
       <c r="F126" s="7" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="G126" s="10" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="H126" s="7" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="I126" s="2" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
     </row>
     <row r="127" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A127" s="7" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B127" s="7" t="s">
         <v>25</v>
@@ -8579,19 +8489,19 @@
       </c>
       <c r="D127" s="7"/>
       <c r="E127" s="7" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="F127" s="7" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="G127" s="10" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="H127" s="7" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="I127" s="2" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
     </row>
     <row r="128" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -8599,14 +8509,14 @@
         <v>170</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="C128" s="7" t="s">
         <v>163</v>
       </c>
       <c r="D128" s="7"/>
       <c r="E128" s="7" t="s">
-        <v>747</v>
+        <v>741</v>
       </c>
       <c r="F128" s="7" t="s">
         <v>171</v>
@@ -8618,7 +8528,7 @@
         <v>173</v>
       </c>
       <c r="I128" s="2" t="s">
-        <v>798</v>
+        <v>792</v>
       </c>
     </row>
     <row r="129" spans="1:27" ht="15" x14ac:dyDescent="0.2">
@@ -8626,26 +8536,26 @@
         <v>196</v>
       </c>
       <c r="B129" s="7" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="C129" s="7" t="s">
         <v>163</v>
       </c>
       <c r="D129" s="7"/>
       <c r="E129" s="7" t="s">
-        <v>748</v>
+        <v>742</v>
       </c>
       <c r="F129" s="7" t="s">
         <v>197</v>
       </c>
       <c r="G129" s="10" t="s">
-        <v>754</v>
+        <v>748</v>
       </c>
       <c r="H129" s="7" t="s">
         <v>198</v>
       </c>
       <c r="I129" s="3" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
     </row>
     <row r="130" spans="1:27" ht="15" x14ac:dyDescent="0.2">
@@ -8660,19 +8570,19 @@
       </c>
       <c r="D130" s="7"/>
       <c r="E130" s="7" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="F130" s="7" t="s">
         <v>64</v>
       </c>
       <c r="G130" s="10" t="s">
-        <v>765</v>
+        <v>759</v>
       </c>
       <c r="H130" s="7" t="s">
         <v>65</v>
       </c>
       <c r="I130" s="2" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="131" spans="1:27" ht="15" x14ac:dyDescent="0.2">
@@ -8687,19 +8597,19 @@
       </c>
       <c r="D131" s="7"/>
       <c r="E131" s="7" t="s">
-        <v>726</v>
+        <v>720</v>
       </c>
       <c r="F131" s="7" t="s">
         <v>43</v>
       </c>
       <c r="G131" s="10" t="s">
-        <v>751</v>
+        <v>745</v>
       </c>
       <c r="H131" s="7" t="s">
         <v>44</v>
       </c>
       <c r="I131" s="2" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="132" spans="1:27" ht="15" x14ac:dyDescent="0.2">
@@ -8714,19 +8624,19 @@
       </c>
       <c r="D132" s="7"/>
       <c r="E132" s="7" t="s">
-        <v>729</v>
+        <v>723</v>
       </c>
       <c r="F132" s="7" t="s">
         <v>109</v>
       </c>
       <c r="G132" s="10" t="s">
-        <v>764</v>
+        <v>758</v>
       </c>
       <c r="H132" s="7" t="s">
         <v>110</v>
       </c>
       <c r="I132" s="2" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="133" spans="1:27" ht="15" x14ac:dyDescent="0.2">
@@ -8734,26 +8644,26 @@
         <v>186</v>
       </c>
       <c r="B133" s="7" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="C133" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D133" s="7"/>
       <c r="E133" s="7" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="F133" s="7" t="s">
         <v>187</v>
       </c>
       <c r="G133" s="10" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="H133" s="7" t="s">
         <v>188</v>
       </c>
       <c r="I133" s="2" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
     </row>
     <row r="134" spans="1:27" ht="15" x14ac:dyDescent="0.2">
@@ -8761,14 +8671,14 @@
         <v>243</v>
       </c>
       <c r="B134" s="7" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="C134" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D134" s="7"/>
       <c r="E134" s="7" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="F134" s="7" t="s">
         <v>241</v>
@@ -8780,34 +8690,34 @@
         <v>244</v>
       </c>
       <c r="I134" s="2" t="s">
-        <v>798</v>
+        <v>792</v>
       </c>
     </row>
     <row r="135" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A135" s="7" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="B135" s="7" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="C135" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D135" s="7"/>
       <c r="E135" s="7" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="F135" s="7" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="G135" s="10" t="s">
-        <v>754</v>
+        <v>748</v>
       </c>
       <c r="H135" s="7" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="I135" s="3" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="J135" s="14"/>
       <c r="K135" s="14"/>
@@ -8830,7 +8740,7 @@
     </row>
     <row r="136" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A136" s="7" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="B136" s="7" t="s">
         <v>25</v>
@@ -8840,24 +8750,24 @@
       </c>
       <c r="D136" s="7"/>
       <c r="E136" s="7" t="s">
-        <v>731</v>
+        <v>725</v>
       </c>
       <c r="F136" s="7" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="G136" s="10" t="s">
-        <v>767</v>
+        <v>761</v>
       </c>
       <c r="H136" s="7" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="I136" s="2" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="137" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A137" s="7" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B137" s="7" t="s">
         <v>25</v>
@@ -8867,19 +8777,19 @@
       </c>
       <c r="D137" s="7"/>
       <c r="E137" s="7" t="s">
-        <v>707</v>
+        <v>702</v>
       </c>
       <c r="F137" s="7" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="G137" s="10" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="H137" s="7" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="I137" s="2" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
     </row>
     <row r="138" spans="1:27" ht="15" x14ac:dyDescent="0.2">
@@ -8894,10 +8804,10 @@
       </c>
       <c r="D138" s="7"/>
       <c r="E138" s="7" t="s">
-        <v>743</v>
+        <v>737</v>
       </c>
       <c r="F138" s="7" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="G138" s="10" t="s">
         <v>257</v>
@@ -8906,12 +8816,12 @@
         <v>258</v>
       </c>
       <c r="I138" s="2" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
     </row>
     <row r="139" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A139" s="7" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B139" s="7" t="s">
         <v>25</v>
@@ -8921,24 +8831,24 @@
       </c>
       <c r="D139" s="7"/>
       <c r="E139" s="7" t="s">
-        <v>703</v>
+        <v>698</v>
       </c>
       <c r="F139" s="7" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="G139" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="H139" s="7" t="s">
         <v>328</v>
       </c>
-      <c r="H139" s="7" t="s">
-        <v>332</v>
-      </c>
       <c r="I139" s="2" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="140" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A140" s="7" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="B140" s="7" t="s">
         <v>25</v>
@@ -8948,19 +8858,19 @@
       </c>
       <c r="D140" s="7"/>
       <c r="E140" s="7" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
       <c r="F140" s="7" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="G140" s="10" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="H140" s="7" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="I140" s="2" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="141" spans="1:27" ht="15" x14ac:dyDescent="0.2">
@@ -8975,7 +8885,7 @@
       </c>
       <c r="D141" s="7"/>
       <c r="E141" s="7" t="s">
-        <v>744</v>
+        <v>738</v>
       </c>
       <c r="F141" s="7" t="s">
         <v>154</v>
@@ -8987,7 +8897,7 @@
         <v>156</v>
       </c>
       <c r="I141" s="2" t="s">
-        <v>793</v>
+        <v>787</v>
       </c>
     </row>
     <row r="142" spans="1:27" ht="15" x14ac:dyDescent="0.2">
@@ -9002,7 +8912,7 @@
       </c>
       <c r="D142" s="7"/>
       <c r="E142" s="7" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="F142" s="7" t="s">
         <v>260</v>
@@ -9014,12 +8924,12 @@
         <v>262</v>
       </c>
       <c r="I142" s="2" t="s">
-        <v>793</v>
+        <v>787</v>
       </c>
     </row>
     <row r="143" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A143" s="7" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B143" s="7" t="s">
         <v>25</v>
@@ -9029,24 +8939,24 @@
       </c>
       <c r="D143" s="7"/>
       <c r="E143" s="7" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="F143" s="7" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="G143" s="10" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="H143" s="7" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="I143" s="2" t="s">
-        <v>793</v>
+        <v>787</v>
       </c>
     </row>
     <row r="144" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A144" s="7" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="B144" s="7" t="s">
         <v>25</v>
@@ -9056,24 +8966,24 @@
       </c>
       <c r="D144" s="7"/>
       <c r="E144" s="7" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="F144" s="7" t="s">
+        <v>508</v>
+      </c>
+      <c r="G144" s="10" t="s">
+        <v>510</v>
+      </c>
+      <c r="H144" s="7" t="s">
         <v>512</v>
       </c>
-      <c r="G144" s="10" t="s">
-        <v>514</v>
-      </c>
-      <c r="H144" s="7" t="s">
-        <v>516</v>
-      </c>
       <c r="I144" s="2" t="s">
-        <v>793</v>
+        <v>787</v>
       </c>
     </row>
     <row r="145" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A145" s="7" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="B145" s="7" t="s">
         <v>25</v>
@@ -9083,19 +8993,19 @@
       </c>
       <c r="D145" s="7"/>
       <c r="E145" s="7" t="s">
-        <v>745</v>
+        <v>739</v>
       </c>
       <c r="F145" s="7" t="s">
+        <v>509</v>
+      </c>
+      <c r="G145" s="10" t="s">
+        <v>511</v>
+      </c>
+      <c r="H145" s="7" t="s">
         <v>513</v>
       </c>
-      <c r="G145" s="10" t="s">
-        <v>515</v>
-      </c>
-      <c r="H145" s="7" t="s">
-        <v>517</v>
-      </c>
       <c r="I145" s="2" t="s">
-        <v>793</v>
+        <v>787</v>
       </c>
     </row>
     <row r="146" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -9110,7 +9020,7 @@
       </c>
       <c r="D146" s="7"/>
       <c r="E146" s="7" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="F146" s="7" t="s">
         <v>56</v>
@@ -9122,7 +9032,7 @@
         <v>58</v>
       </c>
       <c r="I146" s="2" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
     </row>
     <row r="147" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -9137,7 +9047,7 @@
       </c>
       <c r="D147" s="7"/>
       <c r="E147" s="7" t="s">
-        <v>710</v>
+        <v>705</v>
       </c>
       <c r="F147" s="7" t="s">
         <v>115</v>
@@ -9149,12 +9059,12 @@
         <v>117</v>
       </c>
       <c r="I147" s="2" t="s">
-        <v>806</v>
+        <v>800</v>
       </c>
     </row>
     <row r="148" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A148" s="7" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B148" s="7" t="s">
         <v>25</v>
@@ -9164,19 +9074,19 @@
       </c>
       <c r="D148" s="7"/>
       <c r="E148" s="7" t="s">
-        <v>711</v>
+        <v>706</v>
       </c>
       <c r="F148" s="7" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="G148" s="10" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="H148" s="7" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="I148" s="2" t="s">
-        <v>806</v>
+        <v>800</v>
       </c>
     </row>
     <row r="149" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -9191,19 +9101,19 @@
       </c>
       <c r="D149" s="7"/>
       <c r="E149" s="7" t="s">
-        <v>712</v>
+        <v>707</v>
       </c>
       <c r="F149" s="7" t="s">
         <v>246</v>
       </c>
       <c r="G149" s="10" t="s">
-        <v>761</v>
+        <v>755</v>
       </c>
       <c r="H149" s="7" t="s">
         <v>247</v>
       </c>
       <c r="I149" s="2" t="s">
-        <v>806</v>
+        <v>800</v>
       </c>
     </row>
     <row r="150" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -9218,19 +9128,19 @@
       </c>
       <c r="D150" s="7"/>
       <c r="E150" s="7" t="s">
-        <v>713</v>
+        <v>708</v>
       </c>
       <c r="F150" s="7" t="s">
         <v>249</v>
       </c>
       <c r="G150" s="10" t="s">
-        <v>762</v>
+        <v>756</v>
       </c>
       <c r="H150" s="7" t="s">
         <v>250</v>
       </c>
       <c r="I150" s="2" t="s">
-        <v>806</v>
+        <v>800</v>
       </c>
     </row>
     <row r="151" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -9245,7 +9155,7 @@
       </c>
       <c r="D151" s="7"/>
       <c r="E151" s="7" t="s">
-        <v>714</v>
+        <v>709</v>
       </c>
       <c r="F151" s="7" t="s">
         <v>252</v>
@@ -9257,7 +9167,7 @@
         <v>254</v>
       </c>
       <c r="I151" s="2" t="s">
-        <v>807</v>
+        <v>801</v>
       </c>
     </row>
     <row r="152" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -9272,7 +9182,7 @@
       </c>
       <c r="D152" s="7"/>
       <c r="E152" s="7" t="s">
-        <v>715</v>
+        <v>710</v>
       </c>
       <c r="F152" s="7" t="s">
         <v>272</v>
@@ -9284,49 +9194,49 @@
         <v>274</v>
       </c>
       <c r="I152" s="2" t="s">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="153" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="7" t="s">
-        <v>283</v>
+        <v>334</v>
       </c>
       <c r="B153" s="7" t="s">
-        <v>621</v>
+        <v>25</v>
       </c>
       <c r="C153" s="7" t="s">
         <v>55</v>
       </c>
       <c r="D153" s="7"/>
       <c r="E153" s="7" t="s">
-        <v>716</v>
+        <v>711</v>
       </c>
       <c r="F153" s="7" t="s">
-        <v>284</v>
+        <v>335</v>
       </c>
       <c r="G153" s="10" t="s">
-        <v>285</v>
+        <v>336</v>
       </c>
       <c r="H153" s="7" t="s">
-        <v>286</v>
+        <v>337</v>
       </c>
       <c r="I153" s="2" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="154" spans="1:9" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A154" s="7" t="s">
         <v>338</v>
       </c>
       <c r="B154" s="7" t="s">
-        <v>25</v>
+        <v>616</v>
       </c>
       <c r="C154" s="7" t="s">
         <v>55</v>
       </c>
       <c r="D154" s="7"/>
       <c r="E154" s="7" t="s">
-        <v>717</v>
+        <v>740</v>
       </c>
       <c r="F154" s="7" t="s">
         <v>339</v>
@@ -9338,39 +9248,39 @@
         <v>341</v>
       </c>
       <c r="I154" s="2" t="s">
-        <v>808</v>
+        <v>596</v>
       </c>
     </row>
     <row r="155" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A155" s="7" t="s">
-        <v>342</v>
+        <v>489</v>
       </c>
       <c r="B155" s="7" t="s">
-        <v>621</v>
+        <v>25</v>
       </c>
       <c r="C155" s="7" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="D155" s="7"/>
       <c r="E155" s="7" t="s">
-        <v>746</v>
+        <v>712</v>
       </c>
       <c r="F155" s="7" t="s">
-        <v>343</v>
+        <v>490</v>
       </c>
       <c r="G155" s="10" t="s">
-        <v>344</v>
+        <v>351</v>
       </c>
       <c r="H155" s="7" t="s">
-        <v>345</v>
+        <v>491</v>
       </c>
       <c r="I155" s="2" t="s">
-        <v>601</v>
+        <v>803</v>
       </c>
     </row>
     <row r="156" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A156" s="7" t="s">
-        <v>493</v>
+        <v>349</v>
       </c>
       <c r="B156" s="7" t="s">
         <v>25</v>
@@ -9380,24 +9290,24 @@
       </c>
       <c r="D156" s="7"/>
       <c r="E156" s="7" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
       <c r="F156" s="7" t="s">
-        <v>494</v>
+        <v>350</v>
       </c>
       <c r="G156" s="10" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="H156" s="7" t="s">
-        <v>495</v>
+        <v>352</v>
       </c>
       <c r="I156" s="2" t="s">
-        <v>809</v>
+        <v>803</v>
       </c>
     </row>
     <row r="157" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A157" s="7" t="s">
-        <v>353</v>
+        <v>67</v>
       </c>
       <c r="B157" s="7" t="s">
         <v>25</v>
@@ -9407,24 +9317,24 @@
       </c>
       <c r="D157" s="7"/>
       <c r="E157" s="7" t="s">
-        <v>719</v>
+        <v>743</v>
       </c>
       <c r="F157" s="7" t="s">
-        <v>354</v>
+        <v>64</v>
       </c>
       <c r="G157" s="10" t="s">
-        <v>355</v>
+        <v>759</v>
       </c>
       <c r="H157" s="7" t="s">
-        <v>356</v>
-      </c>
-      <c r="I157" s="2" t="s">
-        <v>809</v>
+        <v>65</v>
+      </c>
+      <c r="I157" s="3" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="158" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A158" s="7" t="s">
-        <v>67</v>
+        <v>298</v>
       </c>
       <c r="B158" s="7" t="s">
         <v>25</v>
@@ -9434,78 +9344,78 @@
       </c>
       <c r="D158" s="7"/>
       <c r="E158" s="7" t="s">
-        <v>749</v>
+        <v>714</v>
       </c>
       <c r="F158" s="7" t="s">
-        <v>64</v>
+        <v>299</v>
       </c>
       <c r="G158" s="10" t="s">
-        <v>765</v>
+        <v>300</v>
       </c>
       <c r="H158" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="I158" s="3" t="s">
-        <v>559</v>
+        <v>301</v>
+      </c>
+      <c r="I158" s="2" t="s">
+        <v>789</v>
       </c>
     </row>
     <row r="159" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A159" s="7" t="s">
-        <v>302</v>
+        <v>383</v>
       </c>
       <c r="B159" s="7" t="s">
-        <v>25</v>
+        <v>616</v>
       </c>
       <c r="C159" s="7" t="s">
         <v>68</v>
       </c>
       <c r="D159" s="7"/>
       <c r="E159" s="7" t="s">
-        <v>720</v>
+        <v>715</v>
       </c>
       <c r="F159" s="7" t="s">
-        <v>303</v>
+        <v>384</v>
       </c>
       <c r="G159" s="10" t="s">
-        <v>304</v>
+        <v>385</v>
       </c>
       <c r="H159" s="7" t="s">
-        <v>305</v>
+        <v>386</v>
       </c>
       <c r="I159" s="2" t="s">
-        <v>795</v>
+        <v>804</v>
       </c>
     </row>
     <row r="160" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A160" s="7" t="s">
-        <v>387</v>
+        <v>144</v>
       </c>
       <c r="B160" s="7" t="s">
-        <v>621</v>
+        <v>25</v>
       </c>
       <c r="C160" s="7" t="s">
         <v>68</v>
       </c>
       <c r="D160" s="7"/>
       <c r="E160" s="7" t="s">
-        <v>721</v>
+        <v>716</v>
       </c>
       <c r="F160" s="7" t="s">
-        <v>388</v>
+        <v>145</v>
       </c>
       <c r="G160" s="10" t="s">
-        <v>389</v>
+        <v>146</v>
       </c>
       <c r="H160" s="7" t="s">
-        <v>390</v>
+        <v>147</v>
       </c>
       <c r="I160" s="2" t="s">
-        <v>810</v>
+        <v>790</v>
       </c>
     </row>
     <row r="161" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A161" s="7" t="s">
-        <v>144</v>
+        <v>192</v>
       </c>
       <c r="B161" s="7" t="s">
         <v>25</v>
@@ -9515,24 +9425,24 @@
       </c>
       <c r="D161" s="7"/>
       <c r="E161" s="7" t="s">
-        <v>722</v>
+        <v>717</v>
       </c>
       <c r="F161" s="7" t="s">
-        <v>145</v>
+        <v>193</v>
       </c>
       <c r="G161" s="10" t="s">
-        <v>146</v>
+        <v>194</v>
       </c>
       <c r="H161" s="7" t="s">
-        <v>147</v>
+        <v>195</v>
       </c>
       <c r="I161" s="2" t="s">
-        <v>796</v>
+        <v>589</v>
       </c>
     </row>
     <row r="162" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A162" s="7" t="s">
-        <v>192</v>
+        <v>294</v>
       </c>
       <c r="B162" s="7" t="s">
         <v>25</v>
@@ -9542,64 +9452,64 @@
       </c>
       <c r="D162" s="7"/>
       <c r="E162" s="7" t="s">
-        <v>723</v>
+        <v>718</v>
       </c>
       <c r="F162" s="7" t="s">
-        <v>193</v>
+        <v>295</v>
       </c>
       <c r="G162" s="10" t="s">
-        <v>194</v>
+        <v>296</v>
       </c>
       <c r="H162" s="7" t="s">
-        <v>195</v>
+        <v>297</v>
       </c>
       <c r="I162" s="2" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
     </row>
     <row r="163" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A163" s="7" t="s">
-        <v>298</v>
+        <v>445</v>
       </c>
       <c r="B163" s="7" t="s">
-        <v>25</v>
+        <v>616</v>
       </c>
       <c r="C163" s="7" t="s">
         <v>68</v>
       </c>
       <c r="D163" s="7"/>
       <c r="E163" s="7" t="s">
-        <v>724</v>
+        <v>744</v>
       </c>
       <c r="F163" s="7" t="s">
-        <v>299</v>
+        <v>548</v>
       </c>
       <c r="G163" s="10" t="s">
-        <v>300</v>
+        <v>446</v>
       </c>
       <c r="H163" s="7" t="s">
-        <v>301</v>
+        <v>447</v>
       </c>
       <c r="I163" s="2" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
     </row>
     <row r="164" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A164" s="7" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B164" s="7" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="C164" s="7" t="s">
         <v>68</v>
       </c>
       <c r="D164" s="7"/>
       <c r="E164" s="7" t="s">
-        <v>750</v>
+        <v>719</v>
       </c>
       <c r="F164" s="7" t="s">
-        <v>552</v>
+        <v>449</v>
       </c>
       <c r="G164" s="10" t="s">
         <v>450</v>
@@ -9608,35 +9518,13 @@
         <v>451</v>
       </c>
       <c r="I164" s="2" t="s">
-        <v>602</v>
+        <v>591</v>
       </c>
     </row>
     <row r="165" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A165" s="7" t="s">
-        <v>452</v>
-      </c>
-      <c r="B165" s="7" t="s">
-        <v>621</v>
-      </c>
-      <c r="C165" s="7" t="s">
-        <v>68</v>
-      </c>
       <c r="D165" s="7"/>
-      <c r="E165" s="7" t="s">
-        <v>725</v>
-      </c>
-      <c r="F165" s="7" t="s">
-        <v>453</v>
-      </c>
-      <c r="G165" s="10" t="s">
-        <v>454</v>
-      </c>
-      <c r="H165" s="7" t="s">
-        <v>455</v>
-      </c>
-      <c r="I165" s="2" t="s">
-        <v>595</v>
-      </c>
+      <c r="G165" s="10"/>
+      <c r="H165" s="7"/>
     </row>
     <row r="166" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="D166" s="7"/>
@@ -10613,123 +10501,78 @@
       <c r="G360" s="10"/>
       <c r="H360" s="7"/>
     </row>
-    <row r="361" spans="4:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="D361" s="7"/>
-      <c r="G361" s="10"/>
-      <c r="H361" s="7"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:I165" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I165">
-      <sortCondition ref="C1:C165"/>
+  <autoFilter ref="A1:I164" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I164">
+      <sortCondition ref="C1:C164"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="E155 E128:E129 G131:G157 G128:G129 G27 G29 G1:G25 E1:E54">
-    <cfRule type="expression" dxfId="21" priority="19">
+  <conditionalFormatting sqref="E1:E54 G131:G156">
+    <cfRule type="expression" dxfId="13" priority="3">
       <formula>"a1&lt;&gt;'pl list (sorted)'!A1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E27">
-    <cfRule type="expression" dxfId="20" priority="20">
+    <cfRule type="expression" dxfId="12" priority="20">
       <formula>E27&lt;&gt;E27</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="expression" dxfId="19" priority="29">
+    <cfRule type="expression" dxfId="11" priority="29">
       <formula>E34&lt;&gt;E34</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E56:E71 E83:E84 E98:E100 E110:E111 E114 E136 E141:E144">
-    <cfRule type="expression" dxfId="18" priority="33">
+    <cfRule type="expression" dxfId="10" priority="33">
       <formula>"a1&lt;&gt;'pl list (sorted)'!A1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E102:E103">
-    <cfRule type="expression" dxfId="17" priority="32">
+    <cfRule type="expression" dxfId="9" priority="32">
       <formula>"a1&lt;&gt;'pl list (sorted)'!A1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E103">
-    <cfRule type="expression" dxfId="16" priority="31">
+    <cfRule type="expression" dxfId="8" priority="31">
       <formula>E103&lt;&gt;E103</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E130">
-    <cfRule type="expression" dxfId="15" priority="27">
+    <cfRule type="expression" dxfId="7" priority="27">
       <formula>E130&lt;&gt;E130</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E130:E132">
-    <cfRule type="expression" dxfId="14" priority="28">
+  <conditionalFormatting sqref="E157">
+    <cfRule type="expression" dxfId="6" priority="25">
+      <formula>E157&lt;&gt;E157</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="26">
       <formula>"a1&lt;&gt;'pl list (sorted)'!A1"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E158">
-    <cfRule type="expression" dxfId="13" priority="25">
-      <formula>E158&lt;&gt;E158</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="26">
+  <conditionalFormatting sqref="G1:G25">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>"a1&lt;&gt;'pl list (sorted)'!A1"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G33:G34">
-    <cfRule type="expression" dxfId="11" priority="18">
+  <conditionalFormatting sqref="G27:G34">
+    <cfRule type="expression" dxfId="3" priority="11">
       <formula>"a1&lt;&gt;'pl list (sorted)'!A1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G38:G54">
-    <cfRule type="expression" dxfId="10" priority="22">
+    <cfRule type="expression" dxfId="2" priority="22">
       <formula>"a1&lt;&gt;'pl list (sorted)'!A1"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G56:G69 G72:G77 G79:G82 G159:G165">
-    <cfRule type="expression" dxfId="9" priority="24">
+  <conditionalFormatting sqref="G56:G69 G72:G77 G79:G82 G158:G164">
+    <cfRule type="expression" dxfId="1" priority="24">
       <formula>"a1&lt;&gt;'pl list (sorted)'!A1"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G85:G129">
-    <cfRule type="expression" dxfId="8" priority="21">
-      <formula>"a1&lt;&gt;'pl list (sorted)'!A1"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G28">
-    <cfRule type="expression" dxfId="7" priority="17">
-      <formula>"a1&lt;&gt;'pl list (sorted)'!A1"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G30:G31">
-    <cfRule type="expression" dxfId="6" priority="15">
-      <formula>"a1&lt;&gt;'pl list (sorted)'!A1"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G31">
-    <cfRule type="expression" dxfId="5" priority="12">
-      <formula>"a1&lt;&gt;'pl list (sorted)'!A1"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G32">
-    <cfRule type="expression" dxfId="4" priority="11">
-      <formula>"a1&lt;&gt;'pl list (sorted)'!A1"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G22">
-    <cfRule type="expression" dxfId="3" priority="7">
-      <formula>"a1&lt;&gt;'pl list (sorted)'!A1"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E18">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>"a1&lt;&gt;'pl list (sorted)'!A1"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G18">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>"a1&lt;&gt;'pl list (sorted)'!A1"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G24:G25">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="G85:G129 E128:E132 E154">
+    <cfRule type="expression" dxfId="0" priority="19">
       <formula>"a1&lt;&gt;'pl list (sorted)'!A1"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>